<commit_message>
added pSB1C5, added in flanking regions, removed one RBS as wasn't sure on chassis and spacing
</commit_message>
<xml_diff>
--- a/RBS Collection/RBS Collection.xlsx
+++ b/RBS Collection/RBS Collection.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracihaddock/Git/iGEM-distribution/RBS Collection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/RBS Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D239AA6-2FB3-FE42-A644-B014020C7403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1401A2-2D16-5C40-8924-9653940DCA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29640" yWindow="2980" windowWidth="36360" windowHeight="21080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31820" yWindow="180" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ontology Terms'!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7629" uniqueCount="7572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7661" uniqueCount="7580">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22717,27 +22716,12 @@
     <t>Medium strength T7.2 RBS</t>
   </si>
   <si>
-    <t>SpoVG ribosome binding site (RBS) for B. subtilis</t>
-  </si>
-  <si>
     <t>BBa_Z0262</t>
   </si>
   <si>
-    <t>BBa_K143021</t>
-  </si>
-  <si>
-    <t>BBa_K2963006</t>
-  </si>
-  <si>
     <t>Z0262</t>
   </si>
   <si>
-    <t>K143021</t>
-  </si>
-  <si>
-    <t>K2963006</t>
-  </si>
-  <si>
     <t>RBSs in vector</t>
   </si>
   <si>
@@ -22822,7 +22806,46 @@
     <t>gggccc aagttcactt aaaaaggaga tcaacaatga aagcaatttt cgtactgaaa catcttaatc atgcaatgga ggctttct</t>
   </si>
   <si>
-    <t>RBS - recognized by Corynebacterium glutamicum</t>
+    <t>pSB1C5</t>
+  </si>
+  <si>
+    <t>agag aaaggtggtgaa tacta</t>
+  </si>
+  <si>
+    <t>partial BioBrick scar added before and after</t>
+  </si>
+  <si>
+    <t>SpoVG ribosome binding site (RBS) for B. subtilis - K143021</t>
+  </si>
+  <si>
+    <t>SpoVG</t>
+  </si>
+  <si>
+    <t>BBa_B0034_m1, BBa_B0034_m0, BBa_B0033_m0, BBa_B0032_m0, BBa_B0031_m0, BBa_B0030_m0, BBa_Z0262, SpoVG, BCD1, BCD8, BCD12, BCD13</t>
+  </si>
+  <si>
+    <t>D1003</t>
+  </si>
+  <si>
+    <t>D1004</t>
+  </si>
+  <si>
+    <t>D2001</t>
+  </si>
+  <si>
+    <t>D2002</t>
+  </si>
+  <si>
+    <t>Includes BsaI and fusion site</t>
+  </si>
+  <si>
+    <t>L0 RBS 5' Flanking Region</t>
+  </si>
+  <si>
+    <t>L0 RBS 3' Flanking Region</t>
+  </si>
+  <si>
+    <t>Extra nonsense bases for synthesis</t>
   </si>
 </sst>
 </file>
@@ -23261,11 +23284,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -23280,6 +23298,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23490,12 +23513,22 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="Parts and Devices"/>
+      <sheetName val="Libraries and Composites"/>
       <sheetName val="Ontology Terms"/>
       <sheetName val="Organism Terms"/>
+      <sheetName val="Sequence_alteration_terms"/>
+      <sheetName val="data_source"/>
+      <sheetName val="template_information"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -23750,8 +23783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23825,14 +23858,14 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="61" t="s">
         <v>7534</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="55"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="63"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -24077,20 +24110,22 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A15" s="56" t="s">
-        <v>7544</v>
-      </c>
-      <c r="B15" s="57" t="s">
+      <c r="A15" s="53" t="s">
+        <v>7539</v>
+      </c>
+      <c r="B15" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="56" t="s">
-        <v>7545</v>
-      </c>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="57"/>
+      <c r="C15" s="54" t="s">
+        <v>7568</v>
+      </c>
+      <c r="D15" s="54"/>
+      <c r="E15" s="53" t="s">
+        <v>7540</v>
+      </c>
+      <c r="F15" s="54"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="54"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18" t="b">
         <v>0</v>
@@ -24103,24 +24138,26 @@
         <v>22</v>
       </c>
       <c r="M15" s="19" t="s">
-        <v>7546</v>
+        <v>7541</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A16" s="56" t="s">
-        <v>7547</v>
-      </c>
-      <c r="B16" s="57" t="s">
+      <c r="A16" s="53" t="s">
+        <v>7542</v>
+      </c>
+      <c r="B16" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="56" t="s">
-        <v>7548</v>
-      </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="57"/>
+      <c r="C16" s="53" t="s">
+        <v>7568</v>
+      </c>
+      <c r="D16" s="54"/>
+      <c r="E16" s="53" t="s">
+        <v>7543</v>
+      </c>
+      <c r="F16" s="54"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="54"/>
       <c r="I16" s="18"/>
       <c r="J16" s="21" t="b">
         <v>0</v>
@@ -24133,24 +24170,26 @@
         <v>21</v>
       </c>
       <c r="M16" s="41" t="s">
-        <v>7549</v>
+        <v>7544</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="56" t="s">
-        <v>7550</v>
-      </c>
-      <c r="B17" s="57" t="s">
+      <c r="A17" s="53" t="s">
+        <v>7545</v>
+      </c>
+      <c r="B17" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="56" t="s">
-        <v>7551</v>
-      </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
+      <c r="C17" s="54" t="s">
+        <v>7568</v>
+      </c>
+      <c r="D17" s="54"/>
+      <c r="E17" s="53" t="s">
+        <v>7546</v>
+      </c>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18" t="b">
         <v>0</v>
@@ -24163,24 +24202,26 @@
         <v>20</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>7552</v>
+        <v>7547</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="56" t="s">
-        <v>7553</v>
-      </c>
-      <c r="B18" s="57" t="s">
+      <c r="A18" s="53" t="s">
+        <v>7548</v>
+      </c>
+      <c r="B18" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="56" t="s">
-        <v>7554</v>
-      </c>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
+      <c r="C18" s="54" t="s">
+        <v>7568</v>
+      </c>
+      <c r="D18" s="57"/>
+      <c r="E18" s="53" t="s">
+        <v>7549</v>
+      </c>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18" t="b">
         <v>0</v>
@@ -24193,24 +24234,26 @@
         <v>22</v>
       </c>
       <c r="M18" s="41" t="s">
-        <v>7555</v>
+        <v>7550</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="56" t="s">
-        <v>7556</v>
-      </c>
-      <c r="B19" s="57" t="s">
+      <c r="A19" s="53" t="s">
+        <v>7551</v>
+      </c>
+      <c r="B19" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="57"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="56" t="s">
-        <v>7557</v>
-      </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="57"/>
+      <c r="C19" s="54" t="s">
+        <v>7568</v>
+      </c>
+      <c r="D19" s="57"/>
+      <c r="E19" s="53" t="s">
+        <v>7552</v>
+      </c>
+      <c r="F19" s="54"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="54"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18" t="b">
         <v>0</v>
@@ -24223,24 +24266,26 @@
         <v>23</v>
       </c>
       <c r="M19" s="41" t="s">
-        <v>7558</v>
+        <v>7553</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="56" t="s">
-        <v>7559</v>
-      </c>
-      <c r="B20" s="57" t="s">
+      <c r="A20" s="53" t="s">
+        <v>7554</v>
+      </c>
+      <c r="B20" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="57"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="56" t="s">
-        <v>7560</v>
-      </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="57"/>
+      <c r="C20" s="54" t="s">
+        <v>7568</v>
+      </c>
+      <c r="D20" s="57"/>
+      <c r="E20" s="53" t="s">
+        <v>7555</v>
+      </c>
+      <c r="F20" s="54"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="54"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18" t="b">
         <v>0</v>
@@ -24253,28 +24298,18 @@
         <v>24</v>
       </c>
       <c r="M20" s="52" t="s">
-        <v>7561</v>
+        <v>7556</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="56" t="s">
-        <v>7537</v>
-      </c>
-      <c r="B21" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="56" t="s">
-        <v>7535</v>
-      </c>
-      <c r="F21" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="57" t="s">
-        <v>7540</v>
-      </c>
-      <c r="H21" s="57"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18" t="b">
         <v>0</v>
@@ -24289,24 +24324,24 @@
       <c r="M21" s="18"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A22" s="56" t="s">
-        <v>7538</v>
-      </c>
-      <c r="B22" s="57" t="s">
+      <c r="A22" s="53" t="s">
+        <v>7536</v>
+      </c>
+      <c r="B22" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="57"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="56" t="s">
-        <v>7536</v>
-      </c>
-      <c r="F22" s="57" t="s">
+      <c r="C22" s="54"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="53" t="s">
+        <v>7535</v>
+      </c>
+      <c r="F22" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="56" t="s">
-        <v>7541</v>
-      </c>
-      <c r="H22" s="57"/>
+      <c r="G22" s="53" t="s">
+        <v>7537</v>
+      </c>
+      <c r="H22" s="54"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18" t="b">
         <v>0</v>
@@ -24321,24 +24356,22 @@
       <c r="M22" s="18"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A23" s="56" t="s">
-        <v>7539</v>
-      </c>
-      <c r="B23" s="57" t="s">
+      <c r="A23" s="53" t="s">
+        <v>7570</v>
+      </c>
+      <c r="B23" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="56" t="s">
-        <v>7571</v>
-      </c>
-      <c r="F23" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="56" t="s">
-        <v>7542</v>
-      </c>
-      <c r="H23" s="57"/>
+      <c r="C23" s="54" t="s">
+        <v>7568</v>
+      </c>
+      <c r="D23" s="57"/>
+      <c r="E23" s="53" t="s">
+        <v>7569</v>
+      </c>
+      <c r="F23" s="54"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="54"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18" t="b">
         <v>0</v>
@@ -24348,25 +24381,27 @@
       </c>
       <c r="L23" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="18"/>
+        <v>21</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>7567</v>
+      </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="56" t="s">
-        <v>7563</v>
-      </c>
-      <c r="B24" s="57" t="s">
+      <c r="A24" s="53" t="s">
+        <v>7558</v>
+      </c>
+      <c r="B24" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="56" t="s">
-        <v>7564</v>
-      </c>
-      <c r="F24" s="57"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="57"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="53" t="s">
+        <v>7559</v>
+      </c>
+      <c r="F24" s="54"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="54"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18" t="b">
         <v>0</v>
@@ -24379,24 +24414,24 @@
         <v>84</v>
       </c>
       <c r="M24" s="41" t="s">
-        <v>7562</v>
+        <v>7557</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A25" s="56" t="s">
-        <v>7565</v>
-      </c>
-      <c r="B25" s="57" t="s">
+      <c r="A25" s="53" t="s">
+        <v>7560</v>
+      </c>
+      <c r="B25" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="56" t="s">
-        <v>7564</v>
-      </c>
-      <c r="F25" s="57"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="57"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="53" t="s">
+        <v>7559</v>
+      </c>
+      <c r="F25" s="54"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="54"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18" t="b">
         <v>0</v>
@@ -24409,24 +24444,24 @@
         <v>84</v>
       </c>
       <c r="M25" s="41" t="s">
-        <v>7568</v>
+        <v>7563</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A26" s="56" t="s">
-        <v>7566</v>
-      </c>
-      <c r="B26" s="57" t="s">
+      <c r="A26" s="53" t="s">
+        <v>7561</v>
+      </c>
+      <c r="B26" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="56" t="s">
-        <v>7564</v>
-      </c>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="53" t="s">
+        <v>7559</v>
+      </c>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18" t="b">
         <v>0</v>
@@ -24439,24 +24474,24 @@
         <v>84</v>
       </c>
       <c r="M26" s="41" t="s">
-        <v>7569</v>
+        <v>7564</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="56" t="s">
-        <v>7567</v>
-      </c>
-      <c r="B27" s="57" t="s">
+      <c r="A27" s="53" t="s">
+        <v>7562</v>
+      </c>
+      <c r="B27" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="56" t="s">
-        <v>7564</v>
-      </c>
-      <c r="F27" s="57"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="57"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="53" t="s">
+        <v>7559</v>
+      </c>
+      <c r="F27" s="54"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="54"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18" t="b">
         <v>0</v>
@@ -24469,18 +24504,18 @@
         <v>84</v>
       </c>
       <c r="M27" s="41" t="s">
-        <v>7570</v>
+        <v>7565</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="56"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="57"/>
+      <c r="A28" s="53"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="54"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18" t="b">
         <v>0</v>
@@ -24495,14 +24530,14 @@
       <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="56"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="57"/>
+      <c r="A29" s="53"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="54"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18" t="b">
         <v>0</v>
@@ -24517,14 +24552,14 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="56"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="57"/>
+      <c r="A30" s="53"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="54"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18" t="b">
         <v>0</v>
@@ -24539,14 +24574,26 @@
       <c r="M30" s="23"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="56"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="57"/>
+      <c r="A31" s="53" t="s">
+        <v>7574</v>
+      </c>
+      <c r="B31" s="54" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C31" s="54" t="s">
+        <v>7579</v>
+      </c>
+      <c r="D31" s="57"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="53" t="s">
+        <v>7574</v>
+      </c>
+      <c r="H31" s="54" t="s">
+        <v>7417</v>
+      </c>
       <c r="I31" s="18"/>
       <c r="J31" s="18" t="b">
         <v>0</v>
@@ -24561,14 +24608,26 @@
       <c r="M31" s="23"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A32" s="56"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="57"/>
+      <c r="A32" s="53" t="s">
+        <v>7575</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C32" s="54" t="s">
+        <v>7579</v>
+      </c>
+      <c r="D32" s="57"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" s="53" t="s">
+        <v>7575</v>
+      </c>
+      <c r="H32" s="54" t="s">
+        <v>7417</v>
+      </c>
       <c r="I32" s="18"/>
       <c r="J32" s="18" t="b">
         <v>0</v>
@@ -24583,14 +24642,28 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A33" s="56"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="57"/>
+      <c r="A33" s="53" t="s">
+        <v>7572</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C33" s="54" t="s">
+        <v>7576</v>
+      </c>
+      <c r="D33" s="57"/>
+      <c r="E33" s="53" t="s">
+        <v>7577</v>
+      </c>
+      <c r="F33" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="G33" s="53" t="s">
+        <v>7572</v>
+      </c>
+      <c r="H33" s="54" t="s">
+        <v>7417</v>
+      </c>
       <c r="I33" s="18"/>
       <c r="J33" s="18" t="b">
         <v>0</v>
@@ -24605,14 +24678,28 @@
       <c r="M33" s="24"/>
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A34" s="56"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="57"/>
+      <c r="A34" s="53" t="s">
+        <v>7573</v>
+      </c>
+      <c r="B34" s="54" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C34" s="54" t="s">
+        <v>7576</v>
+      </c>
+      <c r="D34" s="57"/>
+      <c r="E34" s="53" t="s">
+        <v>7578</v>
+      </c>
+      <c r="F34" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" s="53" t="s">
+        <v>7573</v>
+      </c>
+      <c r="H34" s="54" t="s">
+        <v>7417</v>
+      </c>
       <c r="I34" s="18"/>
       <c r="J34" s="18" t="b">
         <v>0</v>
@@ -24627,22 +24714,22 @@
       <c r="M34" s="21"/>
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A35" s="61" t="s">
-        <v>7501</v>
-      </c>
-      <c r="B35" s="61" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="61"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="G35" s="63" t="s">
-        <v>7501</v>
-      </c>
-      <c r="H35" s="57"/>
+      <c r="A35" s="58" t="s">
+        <v>7566</v>
+      </c>
+      <c r="B35" s="58" t="s">
+        <v>4473</v>
+      </c>
+      <c r="C35" s="58"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="58" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G35" s="60" t="s">
+        <v>7566</v>
+      </c>
+      <c r="H35" s="54"/>
       <c r="I35" s="41"/>
       <c r="J35" s="18" t="b">
         <v>0</v>
@@ -25692,7 +25779,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>data_source!$B$2:$B$11</xm:f>
@@ -25721,17 +25808,11 @@
           <x14:formula1>
             <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J15:K34 J36:K38</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
-          <x14:formula1>
-            <xm:f>'[Terminators.xlsx]Ontology Terms'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>J35:K35</xm:sqref>
+          <xm:sqref>J15:K38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
-            <xm:f>'[Terminators.xlsx]Organism Terms'!#REF!</xm:f>
+            <xm:f>'/Users/vinoo/_dev/distribution/iGEM-distribution/Terminators/[Terminators.xlsx]Organism Terms'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>H35:I35</xm:sqref>
         </x14:dataValidation>
@@ -25746,7 +25827,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -26240,22 +26321,32 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" s="52" t="s">
-        <v>7543</v>
+        <v>7538</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="21" t="b">
+      <c r="D14" s="18" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>7501</v>
+        <v>7566</v>
       </c>
       <c r="F14" s="18"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
+      <c r="G14" s="52" t="s">
+        <v>7574</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>7572</v>
+      </c>
+      <c r="I14" s="32" t="s">
+        <v>7571</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>7573</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>7575</v>
+      </c>
       <c r="L14" s="18"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
@@ -26447,18 +26538,12 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D15:D16</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
-          <x14:formula1>
-            <xm:f>'[Terminators.xlsx]Ontology Terms'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D14</xm:sqref>
+          <xm:sqref>D14:D16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>